<commit_message>
Snowfall update + workspace for instructor
</commit_message>
<xml_diff>
--- a/Data/Transportation/Snowfall.xlsx
+++ b/Data/Transportation/Snowfall.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4001" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4000" uniqueCount="13">
   <si>
     <t>StreetId</t>
   </si>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3996"/>
+  <dimension ref="A1:F3995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A3818" workbookViewId="0">
+      <selection activeCell="A3841" sqref="A3841:XFD3841"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -76555,16 +76555,16 @@
     </row>
     <row r="3841" spans="1:6">
       <c r="A3841">
-        <v>12032</v>
+        <v>12036</v>
       </c>
       <c r="B3841">
-        <v>73</v>
+        <v>114</v>
       </c>
       <c r="C3841">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D3841">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3841">
         <v>24</v>
@@ -76575,16 +76575,16 @@
     </row>
     <row r="3842" spans="1:6">
       <c r="A3842">
-        <v>12036</v>
+        <v>12041</v>
       </c>
       <c r="B3842">
-        <v>114</v>
+        <v>187</v>
       </c>
       <c r="C3842">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D3842">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3842">
         <v>24</v>
@@ -76595,16 +76595,16 @@
     </row>
     <row r="3843" spans="1:6">
       <c r="A3843">
-        <v>12041</v>
+        <v>12045</v>
       </c>
       <c r="B3843">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C3843">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D3843">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3843">
         <v>24</v>
@@ -76615,10 +76615,10 @@
     </row>
     <row r="3844" spans="1:6">
       <c r="A3844">
-        <v>12045</v>
+        <v>12067</v>
       </c>
       <c r="B3844">
-        <v>181</v>
+        <v>225</v>
       </c>
       <c r="C3844">
         <v>0.6</v>
@@ -76635,16 +76635,16 @@
     </row>
     <row r="3845" spans="1:6">
       <c r="A3845">
-        <v>12067</v>
+        <v>12134</v>
       </c>
       <c r="B3845">
-        <v>225</v>
+        <v>65</v>
       </c>
       <c r="C3845">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D3845">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E3845">
         <v>24</v>
@@ -76655,10 +76655,10 @@
     </row>
     <row r="3846" spans="1:6">
       <c r="A3846">
-        <v>12134</v>
+        <v>12135</v>
       </c>
       <c r="B3846">
-        <v>65</v>
+        <v>218</v>
       </c>
       <c r="C3846">
         <v>0.4</v>
@@ -76675,10 +76675,10 @@
     </row>
     <row r="3847" spans="1:6">
       <c r="A3847">
-        <v>12135</v>
+        <v>12151</v>
       </c>
       <c r="B3847">
-        <v>218</v>
+        <v>120</v>
       </c>
       <c r="C3847">
         <v>0.4</v>
@@ -76695,10 +76695,10 @@
     </row>
     <row r="3848" spans="1:6">
       <c r="A3848">
-        <v>12151</v>
+        <v>12154</v>
       </c>
       <c r="B3848">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C3848">
         <v>0.4</v>
@@ -76715,10 +76715,10 @@
     </row>
     <row r="3849" spans="1:6">
       <c r="A3849">
-        <v>12154</v>
+        <v>12155</v>
       </c>
       <c r="B3849">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="C3849">
         <v>0.4</v>
@@ -76735,16 +76735,16 @@
     </row>
     <row r="3850" spans="1:6">
       <c r="A3850">
-        <v>12155</v>
+        <v>12204</v>
       </c>
       <c r="B3850">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C3850">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3850">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3850">
         <v>24</v>
@@ -76755,10 +76755,10 @@
     </row>
     <row r="3851" spans="1:6">
       <c r="A3851">
-        <v>12204</v>
+        <v>12205</v>
       </c>
       <c r="B3851">
-        <v>106</v>
+        <v>203</v>
       </c>
       <c r="C3851">
         <v>0.9</v>
@@ -76775,16 +76775,16 @@
     </row>
     <row r="3852" spans="1:6">
       <c r="A3852">
-        <v>12205</v>
+        <v>12243</v>
       </c>
       <c r="B3852">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="C3852">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D3852">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3852">
         <v>24</v>
@@ -76795,16 +76795,16 @@
     </row>
     <row r="3853" spans="1:6">
       <c r="A3853">
-        <v>12243</v>
+        <v>12253</v>
       </c>
       <c r="B3853">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="C3853">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3853">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3853">
         <v>24</v>
@@ -76815,10 +76815,10 @@
     </row>
     <row r="3854" spans="1:6">
       <c r="A3854">
-        <v>12253</v>
+        <v>12254</v>
       </c>
       <c r="B3854">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="C3854">
         <v>0.4</v>
@@ -76835,10 +76835,10 @@
     </row>
     <row r="3855" spans="1:6">
       <c r="A3855">
-        <v>12254</v>
+        <v>12257</v>
       </c>
       <c r="B3855">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="C3855">
         <v>0.4</v>
@@ -76855,10 +76855,10 @@
     </row>
     <row r="3856" spans="1:6">
       <c r="A3856">
-        <v>12257</v>
+        <v>12268</v>
       </c>
       <c r="B3856">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="C3856">
         <v>0.4</v>
@@ -76875,16 +76875,16 @@
     </row>
     <row r="3857" spans="1:6">
       <c r="A3857">
-        <v>12268</v>
+        <v>12298</v>
       </c>
       <c r="B3857">
-        <v>204</v>
+        <v>107</v>
       </c>
       <c r="C3857">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3857">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3857">
         <v>24</v>
@@ -76895,10 +76895,10 @@
     </row>
     <row r="3858" spans="1:6">
       <c r="A3858">
-        <v>12298</v>
+        <v>12299</v>
       </c>
       <c r="B3858">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="C3858">
         <v>0.9</v>
@@ -76915,16 +76915,16 @@
     </row>
     <row r="3859" spans="1:6">
       <c r="A3859">
-        <v>12299</v>
+        <v>12317</v>
       </c>
       <c r="B3859">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="C3859">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D3859">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3859">
         <v>24</v>
@@ -76935,16 +76935,16 @@
     </row>
     <row r="3860" spans="1:6">
       <c r="A3860">
-        <v>12317</v>
+        <v>12322</v>
       </c>
       <c r="B3860">
-        <v>187</v>
+        <v>154</v>
       </c>
       <c r="C3860">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3860">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3860">
         <v>24</v>
@@ -76955,10 +76955,10 @@
     </row>
     <row r="3861" spans="1:6">
       <c r="A3861">
-        <v>12322</v>
+        <v>12358</v>
       </c>
       <c r="B3861">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="C3861">
         <v>0.4</v>
@@ -76975,16 +76975,16 @@
     </row>
     <row r="3862" spans="1:6">
       <c r="A3862">
-        <v>12358</v>
+        <v>12362</v>
       </c>
       <c r="B3862">
-        <v>87</v>
+        <v>225</v>
       </c>
       <c r="C3862">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3862">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3862">
         <v>24</v>
@@ -76995,16 +76995,16 @@
     </row>
     <row r="3863" spans="1:6">
       <c r="A3863">
-        <v>12362</v>
+        <v>12368</v>
       </c>
       <c r="B3863">
-        <v>225</v>
+        <v>178</v>
       </c>
       <c r="C3863">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3863">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3863">
         <v>24</v>
@@ -77015,10 +77015,10 @@
     </row>
     <row r="3864" spans="1:6">
       <c r="A3864">
-        <v>12368</v>
+        <v>12383</v>
       </c>
       <c r="B3864">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="C3864">
         <v>0.4</v>
@@ -77035,10 +77035,10 @@
     </row>
     <row r="3865" spans="1:6">
       <c r="A3865">
-        <v>12383</v>
+        <v>12385</v>
       </c>
       <c r="B3865">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="C3865">
         <v>0.4</v>
@@ -77055,10 +77055,10 @@
     </row>
     <row r="3866" spans="1:6">
       <c r="A3866">
-        <v>12385</v>
+        <v>12386</v>
       </c>
       <c r="B3866">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C3866">
         <v>0.4</v>
@@ -77075,16 +77075,16 @@
     </row>
     <row r="3867" spans="1:6">
       <c r="A3867">
-        <v>12386</v>
+        <v>12441</v>
       </c>
       <c r="B3867">
-        <v>203</v>
+        <v>142</v>
       </c>
       <c r="C3867">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3867">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3867">
         <v>24</v>
@@ -77095,10 +77095,10 @@
     </row>
     <row r="3868" spans="1:6">
       <c r="A3868">
-        <v>12441</v>
+        <v>12442</v>
       </c>
       <c r="B3868">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="C3868">
         <v>0.9</v>
@@ -77115,16 +77115,16 @@
     </row>
     <row r="3869" spans="1:6">
       <c r="A3869">
-        <v>12442</v>
+        <v>12494</v>
       </c>
       <c r="B3869">
-        <v>179</v>
+        <v>232</v>
       </c>
       <c r="C3869">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D3869">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3869">
         <v>24</v>
@@ -77135,16 +77135,16 @@
     </row>
     <row r="3870" spans="1:6">
       <c r="A3870">
-        <v>12494</v>
+        <v>12497</v>
       </c>
       <c r="B3870">
-        <v>232</v>
+        <v>67</v>
       </c>
       <c r="C3870">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D3870">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E3870">
         <v>24</v>
@@ -77155,16 +77155,16 @@
     </row>
     <row r="3871" spans="1:6">
       <c r="A3871">
-        <v>12497</v>
+        <v>12527</v>
       </c>
       <c r="B3871">
-        <v>67</v>
+        <v>239</v>
       </c>
       <c r="C3871">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D3871">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E3871">
         <v>24</v>
@@ -77175,16 +77175,16 @@
     </row>
     <row r="3872" spans="1:6">
       <c r="A3872">
-        <v>12527</v>
+        <v>12550</v>
       </c>
       <c r="B3872">
-        <v>239</v>
+        <v>183</v>
       </c>
       <c r="C3872">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D3872">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E3872">
         <v>24</v>
@@ -77195,10 +77195,10 @@
     </row>
     <row r="3873" spans="1:6">
       <c r="A3873">
-        <v>12550</v>
+        <v>12572</v>
       </c>
       <c r="B3873">
-        <v>183</v>
+        <v>76</v>
       </c>
       <c r="C3873">
         <v>0.4</v>
@@ -77215,10 +77215,10 @@
     </row>
     <row r="3874" spans="1:6">
       <c r="A3874">
-        <v>12572</v>
+        <v>12573</v>
       </c>
       <c r="B3874">
-        <v>76</v>
+        <v>174</v>
       </c>
       <c r="C3874">
         <v>0.4</v>
@@ -77235,10 +77235,10 @@
     </row>
     <row r="3875" spans="1:6">
       <c r="A3875">
-        <v>12573</v>
+        <v>12577</v>
       </c>
       <c r="B3875">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C3875">
         <v>0.4</v>
@@ -77255,16 +77255,16 @@
     </row>
     <row r="3876" spans="1:6">
       <c r="A3876">
-        <v>12577</v>
+        <v>12695</v>
       </c>
       <c r="B3876">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="C3876">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3876">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3876">
         <v>24</v>
@@ -77275,16 +77275,16 @@
     </row>
     <row r="3877" spans="1:6">
       <c r="A3877">
-        <v>12695</v>
+        <v>12697</v>
       </c>
       <c r="B3877">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C3877">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3877">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3877">
         <v>24</v>
@@ -77295,10 +77295,10 @@
     </row>
     <row r="3878" spans="1:6">
       <c r="A3878">
-        <v>12697</v>
+        <v>12707</v>
       </c>
       <c r="B3878">
-        <v>206</v>
+        <v>164</v>
       </c>
       <c r="C3878">
         <v>0.4</v>
@@ -77315,10 +77315,10 @@
     </row>
     <row r="3879" spans="1:6">
       <c r="A3879">
-        <v>12707</v>
+        <v>12709</v>
       </c>
       <c r="B3879">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="C3879">
         <v>0.4</v>
@@ -77335,10 +77335,10 @@
     </row>
     <row r="3880" spans="1:6">
       <c r="A3880">
-        <v>12709</v>
+        <v>12710</v>
       </c>
       <c r="B3880">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="C3880">
         <v>0.4</v>
@@ -77355,10 +77355,10 @@
     </row>
     <row r="3881" spans="1:6">
       <c r="A3881">
-        <v>12710</v>
+        <v>12712</v>
       </c>
       <c r="B3881">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="C3881">
         <v>0.4</v>
@@ -77375,10 +77375,10 @@
     </row>
     <row r="3882" spans="1:6">
       <c r="A3882">
-        <v>12712</v>
+        <v>12715</v>
       </c>
       <c r="B3882">
-        <v>128</v>
+        <v>200</v>
       </c>
       <c r="C3882">
         <v>0.4</v>
@@ -77395,10 +77395,10 @@
     </row>
     <row r="3883" spans="1:6">
       <c r="A3883">
-        <v>12715</v>
+        <v>12722</v>
       </c>
       <c r="B3883">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="C3883">
         <v>0.4</v>
@@ -77415,16 +77415,16 @@
     </row>
     <row r="3884" spans="1:6">
       <c r="A3884">
-        <v>12722</v>
+        <v>12732</v>
       </c>
       <c r="B3884">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C3884">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D3884">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3884">
         <v>24</v>
@@ -77435,16 +77435,16 @@
     </row>
     <row r="3885" spans="1:6">
       <c r="A3885">
-        <v>12732</v>
+        <v>12733</v>
       </c>
       <c r="B3885">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C3885">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3885">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3885">
         <v>24</v>
@@ -77455,16 +77455,16 @@
     </row>
     <row r="3886" spans="1:6">
       <c r="A3886">
-        <v>12733</v>
+        <v>12753</v>
       </c>
       <c r="B3886">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="C3886">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D3886">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E3886">
         <v>24</v>
@@ -77475,16 +77475,16 @@
     </row>
     <row r="3887" spans="1:6">
       <c r="A3887">
-        <v>12753</v>
+        <v>12805</v>
       </c>
       <c r="B3887">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="C3887">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D3887">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3887">
         <v>24</v>
@@ -77495,10 +77495,10 @@
     </row>
     <row r="3888" spans="1:6">
       <c r="A3888">
-        <v>12805</v>
+        <v>12806</v>
       </c>
       <c r="B3888">
-        <v>129</v>
+        <v>187</v>
       </c>
       <c r="C3888">
         <v>0.9</v>
@@ -77515,16 +77515,16 @@
     </row>
     <row r="3889" spans="1:6">
       <c r="A3889">
-        <v>12806</v>
+        <v>12819</v>
       </c>
       <c r="B3889">
-        <v>187</v>
+        <v>122</v>
       </c>
       <c r="C3889">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3889">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3889">
         <v>24</v>
@@ -77535,10 +77535,10 @@
     </row>
     <row r="3890" spans="1:6">
       <c r="A3890">
-        <v>12819</v>
+        <v>12820</v>
       </c>
       <c r="B3890">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="C3890">
         <v>0.4</v>
@@ -77555,16 +77555,16 @@
     </row>
     <row r="3891" spans="1:6">
       <c r="A3891">
-        <v>12820</v>
+        <v>12828</v>
       </c>
       <c r="B3891">
-        <v>57</v>
+        <v>237</v>
       </c>
       <c r="C3891">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3891">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3891">
         <v>24</v>
@@ -77575,16 +77575,16 @@
     </row>
     <row r="3892" spans="1:6">
       <c r="A3892">
-        <v>12828</v>
+        <v>12831</v>
       </c>
       <c r="B3892">
-        <v>237</v>
+        <v>103</v>
       </c>
       <c r="C3892">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D3892">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3892">
         <v>24</v>
@@ -77595,10 +77595,10 @@
     </row>
     <row r="3893" spans="1:6">
       <c r="A3893">
-        <v>12831</v>
+        <v>12836</v>
       </c>
       <c r="B3893">
-        <v>103</v>
+        <v>185</v>
       </c>
       <c r="C3893">
         <v>0.8</v>
@@ -77615,16 +77615,16 @@
     </row>
     <row r="3894" spans="1:6">
       <c r="A3894">
-        <v>12836</v>
+        <v>12839</v>
       </c>
       <c r="B3894">
-        <v>185</v>
+        <v>93</v>
       </c>
       <c r="C3894">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3894">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3894">
         <v>24</v>
@@ -77635,10 +77635,10 @@
     </row>
     <row r="3895" spans="1:6">
       <c r="A3895">
-        <v>12839</v>
+        <v>12840</v>
       </c>
       <c r="B3895">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="C3895">
         <v>0.4</v>
@@ -77655,10 +77655,10 @@
     </row>
     <row r="3896" spans="1:6">
       <c r="A3896">
-        <v>12840</v>
+        <v>12882</v>
       </c>
       <c r="B3896">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C3896">
         <v>0.4</v>
@@ -77675,10 +77675,10 @@
     </row>
     <row r="3897" spans="1:6">
       <c r="A3897">
-        <v>12882</v>
+        <v>12901</v>
       </c>
       <c r="B3897">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="C3897">
         <v>0.4</v>
@@ -77695,10 +77695,10 @@
     </row>
     <row r="3898" spans="1:6">
       <c r="A3898">
-        <v>12901</v>
+        <v>12936</v>
       </c>
       <c r="B3898">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C3898">
         <v>0.4</v>
@@ -77715,16 +77715,16 @@
     </row>
     <row r="3899" spans="1:6">
       <c r="A3899">
-        <v>12936</v>
+        <v>12945</v>
       </c>
       <c r="B3899">
-        <v>99</v>
+        <v>131</v>
       </c>
       <c r="C3899">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3899">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3899">
         <v>24</v>
@@ -77735,16 +77735,16 @@
     </row>
     <row r="3900" spans="1:6">
       <c r="A3900">
-        <v>12945</v>
+        <v>12985</v>
       </c>
       <c r="B3900">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="C3900">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D3900">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3900">
         <v>24</v>
@@ -77755,16 +77755,16 @@
     </row>
     <row r="3901" spans="1:6">
       <c r="A3901">
-        <v>12985</v>
+        <v>13002</v>
       </c>
       <c r="B3901">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="C3901">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D3901">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E3901">
         <v>24</v>
@@ -77775,10 +77775,10 @@
     </row>
     <row r="3902" spans="1:6">
       <c r="A3902">
-        <v>13002</v>
+        <v>13006</v>
       </c>
       <c r="B3902">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="C3902">
         <v>0.4</v>
@@ -77795,10 +77795,10 @@
     </row>
     <row r="3903" spans="1:6">
       <c r="A3903">
-        <v>13006</v>
+        <v>13090</v>
       </c>
       <c r="B3903">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="C3903">
         <v>0.4</v>
@@ -77815,16 +77815,16 @@
     </row>
     <row r="3904" spans="1:6">
       <c r="A3904">
-        <v>13090</v>
+        <v>13165</v>
       </c>
       <c r="B3904">
-        <v>66</v>
+        <v>216</v>
       </c>
       <c r="C3904">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D3904">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3904">
         <v>24</v>
@@ -77835,10 +77835,10 @@
     </row>
     <row r="3905" spans="1:6">
       <c r="A3905">
-        <v>13165</v>
+        <v>13173</v>
       </c>
       <c r="B3905">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C3905">
         <v>0.8</v>
@@ -77855,16 +77855,16 @@
     </row>
     <row r="3906" spans="1:6">
       <c r="A3906">
-        <v>13173</v>
+        <v>13178</v>
       </c>
       <c r="B3906">
-        <v>220</v>
+        <v>114</v>
       </c>
       <c r="C3906">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D3906">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3906">
         <v>24</v>
@@ -77875,16 +77875,16 @@
     </row>
     <row r="3907" spans="1:6">
       <c r="A3907">
-        <v>13178</v>
+        <v>13207</v>
       </c>
       <c r="B3907">
-        <v>114</v>
+        <v>191</v>
       </c>
       <c r="C3907">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3907">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3907">
         <v>24</v>
@@ -77895,10 +77895,10 @@
     </row>
     <row r="3908" spans="1:6">
       <c r="A3908">
-        <v>13207</v>
+        <v>13213</v>
       </c>
       <c r="B3908">
-        <v>191</v>
+        <v>66</v>
       </c>
       <c r="C3908">
         <v>0.4</v>
@@ -77915,10 +77915,10 @@
     </row>
     <row r="3909" spans="1:6">
       <c r="A3909">
-        <v>13213</v>
+        <v>13214</v>
       </c>
       <c r="B3909">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="C3909">
         <v>0.4</v>
@@ -77935,10 +77935,10 @@
     </row>
     <row r="3910" spans="1:6">
       <c r="A3910">
-        <v>13214</v>
+        <v>13223</v>
       </c>
       <c r="B3910">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3910">
         <v>0.4</v>
@@ -77955,16 +77955,16 @@
     </row>
     <row r="3911" spans="1:6">
       <c r="A3911">
-        <v>13223</v>
+        <v>13224</v>
       </c>
       <c r="B3911">
-        <v>159</v>
+        <v>100</v>
       </c>
       <c r="C3911">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3911">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3911">
         <v>24</v>
@@ -77975,16 +77975,16 @@
     </row>
     <row r="3912" spans="1:6">
       <c r="A3912">
-        <v>13224</v>
+        <v>13235</v>
       </c>
       <c r="B3912">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3912">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3912">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3912">
         <v>24</v>
@@ -77995,10 +77995,10 @@
     </row>
     <row r="3913" spans="1:6">
       <c r="A3913">
-        <v>13235</v>
+        <v>13245</v>
       </c>
       <c r="B3913">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C3913">
         <v>0.4</v>
@@ -78015,10 +78015,10 @@
     </row>
     <row r="3914" spans="1:6">
       <c r="A3914">
-        <v>13245</v>
+        <v>13269</v>
       </c>
       <c r="B3914">
-        <v>113</v>
+        <v>199</v>
       </c>
       <c r="C3914">
         <v>0.4</v>
@@ -78035,16 +78035,16 @@
     </row>
     <row r="3915" spans="1:6">
       <c r="A3915">
-        <v>13269</v>
+        <v>13275</v>
       </c>
       <c r="B3915">
-        <v>199</v>
+        <v>103</v>
       </c>
       <c r="C3915">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3915">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3915">
         <v>24</v>
@@ -78055,10 +78055,10 @@
     </row>
     <row r="3916" spans="1:6">
       <c r="A3916">
-        <v>13275</v>
+        <v>13276</v>
       </c>
       <c r="B3916">
-        <v>103</v>
+        <v>192</v>
       </c>
       <c r="C3916">
         <v>0.9</v>
@@ -78075,10 +78075,10 @@
     </row>
     <row r="3917" spans="1:6">
       <c r="A3917">
-        <v>13276</v>
+        <v>13279</v>
       </c>
       <c r="B3917">
-        <v>192</v>
+        <v>149</v>
       </c>
       <c r="C3917">
         <v>0.9</v>
@@ -78095,10 +78095,10 @@
     </row>
     <row r="3918" spans="1:6">
       <c r="A3918">
-        <v>13279</v>
+        <v>13280</v>
       </c>
       <c r="B3918">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="C3918">
         <v>0.9</v>
@@ -78115,10 +78115,10 @@
     </row>
     <row r="3919" spans="1:6">
       <c r="A3919">
-        <v>13280</v>
+        <v>13281</v>
       </c>
       <c r="B3919">
-        <v>183</v>
+        <v>101</v>
       </c>
       <c r="C3919">
         <v>0.9</v>
@@ -78135,16 +78135,16 @@
     </row>
     <row r="3920" spans="1:6">
       <c r="A3920">
-        <v>13281</v>
+        <v>13297</v>
       </c>
       <c r="B3920">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C3920">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3920">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3920">
         <v>24</v>
@@ -78155,16 +78155,16 @@
     </row>
     <row r="3921" spans="1:6">
       <c r="A3921">
-        <v>13297</v>
+        <v>13320</v>
       </c>
       <c r="B3921">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="C3921">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3921">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3921">
         <v>24</v>
@@ -78175,16 +78175,16 @@
     </row>
     <row r="3922" spans="1:6">
       <c r="A3922">
-        <v>13320</v>
+        <v>13380</v>
       </c>
       <c r="B3922">
-        <v>162</v>
+        <v>214</v>
       </c>
       <c r="C3922">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3922">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3922">
         <v>24</v>
@@ -78195,16 +78195,16 @@
     </row>
     <row r="3923" spans="1:6">
       <c r="A3923">
-        <v>13380</v>
+        <v>13409</v>
       </c>
       <c r="B3923">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C3923">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3923">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3923">
         <v>24</v>
@@ -78215,10 +78215,10 @@
     </row>
     <row r="3924" spans="1:6">
       <c r="A3924">
-        <v>13409</v>
+        <v>13410</v>
       </c>
       <c r="B3924">
-        <v>213</v>
+        <v>162</v>
       </c>
       <c r="C3924">
         <v>0.9</v>
@@ -78235,10 +78235,10 @@
     </row>
     <row r="3925" spans="1:6">
       <c r="A3925">
-        <v>13410</v>
+        <v>13411</v>
       </c>
       <c r="B3925">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C3925">
         <v>0.9</v>
@@ -78255,16 +78255,16 @@
     </row>
     <row r="3926" spans="1:6">
       <c r="A3926">
-        <v>13411</v>
+        <v>13415</v>
       </c>
       <c r="B3926">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="C3926">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3926">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3926">
         <v>24</v>
@@ -78275,7 +78275,7 @@
     </row>
     <row r="3927" spans="1:6">
       <c r="A3927">
-        <v>13415</v>
+        <v>13417</v>
       </c>
       <c r="B3927">
         <v>222</v>
@@ -78295,16 +78295,16 @@
     </row>
     <row r="3928" spans="1:6">
       <c r="A3928">
-        <v>13417</v>
+        <v>13552</v>
       </c>
       <c r="B3928">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C3928">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D3928">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E3928">
         <v>24</v>
@@ -78315,16 +78315,16 @@
     </row>
     <row r="3929" spans="1:6">
       <c r="A3929">
-        <v>13552</v>
+        <v>13585</v>
       </c>
       <c r="B3929">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C3929">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D3929">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3929">
         <v>24</v>
@@ -78335,16 +78335,16 @@
     </row>
     <row r="3930" spans="1:6">
       <c r="A3930">
-        <v>13585</v>
+        <v>13589</v>
       </c>
       <c r="B3930">
-        <v>242</v>
+        <v>163</v>
       </c>
       <c r="C3930">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D3930">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3930">
         <v>24</v>
@@ -78355,16 +78355,16 @@
     </row>
     <row r="3931" spans="1:6">
       <c r="A3931">
-        <v>13589</v>
+        <v>13594</v>
       </c>
       <c r="B3931">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C3931">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3931">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3931">
         <v>24</v>
@@ -78375,10 +78375,10 @@
     </row>
     <row r="3932" spans="1:6">
       <c r="A3932">
-        <v>13594</v>
+        <v>13595</v>
       </c>
       <c r="B3932">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C3932">
         <v>0.4</v>
@@ -78395,10 +78395,10 @@
     </row>
     <row r="3933" spans="1:6">
       <c r="A3933">
-        <v>13595</v>
+        <v>13596</v>
       </c>
       <c r="B3933">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="C3933">
         <v>0.4</v>
@@ -78415,10 +78415,10 @@
     </row>
     <row r="3934" spans="1:6">
       <c r="A3934">
-        <v>13596</v>
+        <v>13597</v>
       </c>
       <c r="B3934">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="C3934">
         <v>0.4</v>
@@ -78435,16 +78435,16 @@
     </row>
     <row r="3935" spans="1:6">
       <c r="A3935">
-        <v>13597</v>
+        <v>13621</v>
       </c>
       <c r="B3935">
-        <v>138</v>
+        <v>243</v>
       </c>
       <c r="C3935">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D3935">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3935">
         <v>24</v>
@@ -78455,16 +78455,16 @@
     </row>
     <row r="3936" spans="1:6">
       <c r="A3936">
-        <v>13621</v>
+        <v>13634</v>
       </c>
       <c r="B3936">
-        <v>243</v>
+        <v>140</v>
       </c>
       <c r="C3936">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3936">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3936">
         <v>24</v>
@@ -78475,10 +78475,10 @@
     </row>
     <row r="3937" spans="1:6">
       <c r="A3937">
-        <v>13634</v>
+        <v>13641</v>
       </c>
       <c r="B3937">
-        <v>140</v>
+        <v>207</v>
       </c>
       <c r="C3937">
         <v>0.4</v>
@@ -78495,10 +78495,10 @@
     </row>
     <row r="3938" spans="1:6">
       <c r="A3938">
-        <v>13641</v>
+        <v>13646</v>
       </c>
       <c r="B3938">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C3938">
         <v>0.4</v>
@@ -78515,16 +78515,16 @@
     </row>
     <row r="3939" spans="1:6">
       <c r="A3939">
-        <v>13646</v>
+        <v>13648</v>
       </c>
       <c r="B3939">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C3939">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D3939">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3939">
         <v>24</v>
@@ -78535,16 +78535,16 @@
     </row>
     <row r="3940" spans="1:6">
       <c r="A3940">
-        <v>13648</v>
+        <v>13658</v>
       </c>
       <c r="B3940">
-        <v>205</v>
+        <v>139</v>
       </c>
       <c r="C3940">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3940">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3940">
         <v>24</v>
@@ -78555,16 +78555,16 @@
     </row>
     <row r="3941" spans="1:6">
       <c r="A3941">
-        <v>13658</v>
+        <v>13662</v>
       </c>
       <c r="B3941">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C3941">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3941">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3941">
         <v>24</v>
@@ -78575,16 +78575,16 @@
     </row>
     <row r="3942" spans="1:6">
       <c r="A3942">
-        <v>13662</v>
+        <v>13681</v>
       </c>
       <c r="B3942">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="C3942">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3942">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3942">
         <v>24</v>
@@ -78595,10 +78595,10 @@
     </row>
     <row r="3943" spans="1:6">
       <c r="A3943">
-        <v>13681</v>
+        <v>13682</v>
       </c>
       <c r="B3943">
-        <v>202</v>
+        <v>110</v>
       </c>
       <c r="C3943">
         <v>0.4</v>
@@ -78615,16 +78615,16 @@
     </row>
     <row r="3944" spans="1:6">
       <c r="A3944">
-        <v>13682</v>
+        <v>13690</v>
       </c>
       <c r="B3944">
-        <v>110</v>
+        <v>202</v>
       </c>
       <c r="C3944">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3944">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3944">
         <v>24</v>
@@ -78635,16 +78635,16 @@
     </row>
     <row r="3945" spans="1:6">
       <c r="A3945">
-        <v>13690</v>
+        <v>13722</v>
       </c>
       <c r="B3945">
-        <v>202</v>
+        <v>95</v>
       </c>
       <c r="C3945">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3945">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3945">
         <v>24</v>
@@ -78655,10 +78655,10 @@
     </row>
     <row r="3946" spans="1:6">
       <c r="A3946">
-        <v>13722</v>
+        <v>13844</v>
       </c>
       <c r="B3946">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="C3946">
         <v>0.4</v>
@@ -78675,16 +78675,16 @@
     </row>
     <row r="3947" spans="1:6">
       <c r="A3947">
-        <v>13844</v>
+        <v>13907</v>
       </c>
       <c r="B3947">
-        <v>234</v>
+        <v>96</v>
       </c>
       <c r="C3947">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3947">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3947">
         <v>24</v>
@@ -78695,16 +78695,16 @@
     </row>
     <row r="3948" spans="1:6">
       <c r="A3948">
-        <v>13907</v>
+        <v>13957</v>
       </c>
       <c r="B3948">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C3948">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3948">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3948">
         <v>24</v>
@@ -78715,10 +78715,10 @@
     </row>
     <row r="3949" spans="1:6">
       <c r="A3949">
-        <v>13957</v>
+        <v>13963</v>
       </c>
       <c r="B3949">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="C3949">
         <v>0.4</v>
@@ -78735,10 +78735,10 @@
     </row>
     <row r="3950" spans="1:6">
       <c r="A3950">
-        <v>13963</v>
+        <v>13965</v>
       </c>
       <c r="B3950">
-        <v>147</v>
+        <v>227</v>
       </c>
       <c r="C3950">
         <v>0.4</v>
@@ -78755,10 +78755,10 @@
     </row>
     <row r="3951" spans="1:6">
       <c r="A3951">
-        <v>13965</v>
+        <v>13966</v>
       </c>
       <c r="B3951">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="C3951">
         <v>0.4</v>
@@ -78775,16 +78775,16 @@
     </row>
     <row r="3952" spans="1:6">
       <c r="A3952">
-        <v>13966</v>
+        <v>13987</v>
       </c>
       <c r="B3952">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="C3952">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="D3952">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3952">
         <v>24</v>
@@ -78795,16 +78795,16 @@
     </row>
     <row r="3953" spans="1:6">
       <c r="A3953">
-        <v>13987</v>
+        <v>13992</v>
       </c>
       <c r="B3953">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="C3953">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D3953">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3953">
         <v>24</v>
@@ -78815,16 +78815,16 @@
     </row>
     <row r="3954" spans="1:6">
       <c r="A3954">
-        <v>13992</v>
+        <v>10803</v>
       </c>
       <c r="B3954">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="C3954">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D3954">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3954">
         <v>24</v>
@@ -78835,16 +78835,16 @@
     </row>
     <row r="3955" spans="1:6">
       <c r="A3955">
-        <v>10803</v>
+        <v>12511</v>
       </c>
       <c r="B3955">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C3955">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D3955">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3955">
         <v>24</v>
@@ -78855,16 +78855,16 @@
     </row>
     <row r="3956" spans="1:6">
       <c r="A3956">
-        <v>12511</v>
+        <v>10419</v>
       </c>
       <c r="B3956">
-        <v>32</v>
+        <v>237</v>
       </c>
       <c r="C3956">
-        <v>0.4</v>
+        <v>-0.7</v>
       </c>
       <c r="D3956">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3956">
         <v>24</v>
@@ -78875,10 +78875,10 @@
     </row>
     <row r="3957" spans="1:6">
       <c r="A3957">
-        <v>10419</v>
+        <v>11255</v>
       </c>
       <c r="B3957">
-        <v>237</v>
+        <v>122</v>
       </c>
       <c r="C3957">
         <v>-0.7</v>
@@ -78895,10 +78895,10 @@
     </row>
     <row r="3958" spans="1:6">
       <c r="A3958">
-        <v>11255</v>
+        <v>11547</v>
       </c>
       <c r="B3958">
-        <v>122</v>
+        <v>8</v>
       </c>
       <c r="C3958">
         <v>-0.7</v>
@@ -78915,10 +78915,10 @@
     </row>
     <row r="3959" spans="1:6">
       <c r="A3959">
-        <v>11547</v>
+        <v>11804</v>
       </c>
       <c r="B3959">
-        <v>8</v>
+        <v>235</v>
       </c>
       <c r="C3959">
         <v>-0.7</v>
@@ -78935,10 +78935,10 @@
     </row>
     <row r="3960" spans="1:6">
       <c r="A3960">
-        <v>11804</v>
+        <v>11978</v>
       </c>
       <c r="B3960">
-        <v>235</v>
+        <v>62</v>
       </c>
       <c r="C3960">
         <v>-0.7</v>
@@ -78955,10 +78955,10 @@
     </row>
     <row r="3961" spans="1:6">
       <c r="A3961">
-        <v>11978</v>
+        <v>12004</v>
       </c>
       <c r="B3961">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="C3961">
         <v>-0.7</v>
@@ -78975,10 +78975,10 @@
     </row>
     <row r="3962" spans="1:6">
       <c r="A3962">
-        <v>12004</v>
+        <v>12128</v>
       </c>
       <c r="B3962">
-        <v>121</v>
+        <v>220</v>
       </c>
       <c r="C3962">
         <v>-0.7</v>
@@ -78995,10 +78995,10 @@
     </row>
     <row r="3963" spans="1:6">
       <c r="A3963">
-        <v>12128</v>
+        <v>12512</v>
       </c>
       <c r="B3963">
-        <v>220</v>
+        <v>1</v>
       </c>
       <c r="C3963">
         <v>-0.7</v>
@@ -79015,10 +79015,10 @@
     </row>
     <row r="3964" spans="1:6">
       <c r="A3964">
-        <v>12512</v>
+        <v>12699</v>
       </c>
       <c r="B3964">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C3964">
         <v>-0.7</v>
@@ -79035,10 +79035,10 @@
     </row>
     <row r="3965" spans="1:6">
       <c r="A3965">
-        <v>12699</v>
+        <v>12841</v>
       </c>
       <c r="B3965">
-        <v>74</v>
+        <v>155</v>
       </c>
       <c r="C3965">
         <v>-0.7</v>
@@ -79055,10 +79055,10 @@
     </row>
     <row r="3966" spans="1:6">
       <c r="A3966">
-        <v>12841</v>
+        <v>13401</v>
       </c>
       <c r="B3966">
-        <v>155</v>
+        <v>47</v>
       </c>
       <c r="C3966">
         <v>-0.7</v>
@@ -79075,10 +79075,10 @@
     </row>
     <row r="3967" spans="1:6">
       <c r="A3967">
-        <v>13401</v>
+        <v>13876</v>
       </c>
       <c r="B3967">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C3967">
         <v>-0.7</v>
@@ -79095,10 +79095,10 @@
     </row>
     <row r="3968" spans="1:6">
       <c r="A3968">
-        <v>13876</v>
+        <v>13881</v>
       </c>
       <c r="B3968">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C3968">
         <v>-0.7</v>
@@ -79115,10 +79115,10 @@
     </row>
     <row r="3969" spans="1:6">
       <c r="A3969">
-        <v>13881</v>
+        <v>14050</v>
       </c>
       <c r="B3969">
-        <v>20</v>
+        <v>214</v>
       </c>
       <c r="C3969">
         <v>-0.7</v>
@@ -79135,10 +79135,10 @@
     </row>
     <row r="3970" spans="1:6">
       <c r="A3970">
-        <v>14050</v>
+        <v>14056</v>
       </c>
       <c r="B3970">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="C3970">
         <v>-0.7</v>
@@ -79155,10 +79155,10 @@
     </row>
     <row r="3971" spans="1:6">
       <c r="A3971">
-        <v>14056</v>
+        <v>10870</v>
       </c>
       <c r="B3971">
-        <v>189</v>
+        <v>36</v>
       </c>
       <c r="C3971">
         <v>-0.7</v>
@@ -79175,30 +79175,30 @@
     </row>
     <row r="3972" spans="1:6">
       <c r="A3972">
-        <v>10870</v>
+        <v>11136</v>
       </c>
       <c r="B3972">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C3972">
-        <v>-0.7</v>
+        <v>0.4</v>
       </c>
       <c r="D3972">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3972">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F3972" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3973" spans="1:6">
       <c r="A3973">
-        <v>11136</v>
+        <v>11137</v>
       </c>
       <c r="B3973">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="C3973">
         <v>0.4</v>
@@ -79215,10 +79215,10 @@
     </row>
     <row r="3974" spans="1:6">
       <c r="A3974">
-        <v>11137</v>
+        <v>11549</v>
       </c>
       <c r="B3974">
-        <v>103</v>
+        <v>46</v>
       </c>
       <c r="C3974">
         <v>0.4</v>
@@ -79235,16 +79235,16 @@
     </row>
     <row r="3975" spans="1:6">
       <c r="A3975">
-        <v>11549</v>
+        <v>11576</v>
       </c>
       <c r="B3975">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="C3975">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D3975">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3975">
         <v>12</v>
@@ -79255,16 +79255,16 @@
     </row>
     <row r="3976" spans="1:6">
       <c r="A3976">
-        <v>11576</v>
+        <v>11801</v>
       </c>
       <c r="B3976">
-        <v>206</v>
+        <v>73</v>
       </c>
       <c r="C3976">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D3976">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3976">
         <v>12</v>
@@ -79275,10 +79275,10 @@
     </row>
     <row r="3977" spans="1:6">
       <c r="A3977">
-        <v>11801</v>
+        <v>12549</v>
       </c>
       <c r="B3977">
-        <v>73</v>
+        <v>203</v>
       </c>
       <c r="C3977">
         <v>0.4</v>
@@ -79295,10 +79295,10 @@
     </row>
     <row r="3978" spans="1:6">
       <c r="A3978">
-        <v>12549</v>
+        <v>13013</v>
       </c>
       <c r="B3978">
-        <v>203</v>
+        <v>105</v>
       </c>
       <c r="C3978">
         <v>0.4</v>
@@ -79315,10 +79315,10 @@
     </row>
     <row r="3979" spans="1:6">
       <c r="A3979">
-        <v>13013</v>
+        <v>13014</v>
       </c>
       <c r="B3979">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C3979">
         <v>0.4</v>
@@ -79335,10 +79335,10 @@
     </row>
     <row r="3980" spans="1:6">
       <c r="A3980">
-        <v>13014</v>
+        <v>13802</v>
       </c>
       <c r="B3980">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="C3980">
         <v>0.4</v>
@@ -79355,10 +79355,10 @@
     </row>
     <row r="3981" spans="1:6">
       <c r="A3981">
-        <v>13802</v>
+        <v>12551</v>
       </c>
       <c r="B3981">
-        <v>229</v>
+        <v>112</v>
       </c>
       <c r="C3981">
         <v>0.4</v>
@@ -79375,16 +79375,16 @@
     </row>
     <row r="3982" spans="1:6">
       <c r="A3982">
-        <v>12551</v>
+        <v>11133</v>
       </c>
       <c r="B3982">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="C3982">
-        <v>0.4</v>
+        <v>-0.7</v>
       </c>
       <c r="D3982">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3982">
         <v>12</v>
@@ -79395,10 +79395,10 @@
     </row>
     <row r="3983" spans="1:6">
       <c r="A3983">
-        <v>11133</v>
+        <v>11138</v>
       </c>
       <c r="B3983">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C3983">
         <v>-0.7</v>
@@ -79415,10 +79415,10 @@
     </row>
     <row r="3984" spans="1:6">
       <c r="A3984">
-        <v>11138</v>
+        <v>12552</v>
       </c>
       <c r="B3984">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="C3984">
         <v>-0.7</v>
@@ -79435,10 +79435,10 @@
     </row>
     <row r="3985" spans="1:6">
       <c r="A3985">
-        <v>12552</v>
+        <v>13011</v>
       </c>
       <c r="B3985">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="C3985">
         <v>-0.7</v>
@@ -79455,10 +79455,10 @@
     </row>
     <row r="3986" spans="1:6">
       <c r="A3986">
-        <v>13011</v>
+        <v>13059</v>
       </c>
       <c r="B3986">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3986">
         <v>-0.7</v>
@@ -79475,10 +79475,10 @@
     </row>
     <row r="3987" spans="1:6">
       <c r="A3987">
-        <v>13059</v>
+        <v>13060</v>
       </c>
       <c r="B3987">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C3987">
         <v>-0.7</v>
@@ -79495,10 +79495,10 @@
     </row>
     <row r="3988" spans="1:6">
       <c r="A3988">
-        <v>13060</v>
+        <v>13071</v>
       </c>
       <c r="B3988">
-        <v>147</v>
+        <v>235</v>
       </c>
       <c r="C3988">
         <v>-0.7</v>
@@ -79515,10 +79515,10 @@
     </row>
     <row r="3989" spans="1:6">
       <c r="A3989">
-        <v>13071</v>
+        <v>13098</v>
       </c>
       <c r="B3989">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="C3989">
         <v>-0.7</v>
@@ -79535,10 +79535,10 @@
     </row>
     <row r="3990" spans="1:6">
       <c r="A3990">
-        <v>13098</v>
+        <v>13542</v>
       </c>
       <c r="B3990">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C3990">
         <v>-0.7</v>
@@ -79555,10 +79555,10 @@
     </row>
     <row r="3991" spans="1:6">
       <c r="A3991">
-        <v>13542</v>
+        <v>13543</v>
       </c>
       <c r="B3991">
-        <v>221</v>
+        <v>125</v>
       </c>
       <c r="C3991">
         <v>-0.7</v>
@@ -79575,10 +79575,10 @@
     </row>
     <row r="3992" spans="1:6">
       <c r="A3992">
-        <v>13543</v>
+        <v>13559</v>
       </c>
       <c r="B3992">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C3992">
         <v>-0.7</v>
@@ -79595,10 +79595,10 @@
     </row>
     <row r="3993" spans="1:6">
       <c r="A3993">
-        <v>13559</v>
+        <v>13784</v>
       </c>
       <c r="B3993">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="C3993">
         <v>-0.7</v>
@@ -79615,10 +79615,10 @@
     </row>
     <row r="3994" spans="1:6">
       <c r="A3994">
-        <v>13784</v>
+        <v>13800</v>
       </c>
       <c r="B3994">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="C3994">
         <v>-0.7</v>
@@ -79635,10 +79635,10 @@
     </row>
     <row r="3995" spans="1:6">
       <c r="A3995">
-        <v>13800</v>
+        <v>14060</v>
       </c>
       <c r="B3995">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C3995">
         <v>-0.7</v>
@@ -79650,26 +79650,6 @@
         <v>12</v>
       </c>
       <c r="F3995" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3996" spans="1:6">
-      <c r="A3996">
-        <v>14060</v>
-      </c>
-      <c r="B3996">
-        <v>200</v>
-      </c>
-      <c r="C3996">
-        <v>-0.7</v>
-      </c>
-      <c r="D3996">
-        <v>7</v>
-      </c>
-      <c r="E3996">
-        <v>12</v>
-      </c>
-      <c r="F3996" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>